<commit_message>
70% progress on handling assembleAOperandAndComplexOperand. still got bug on (test/test_instruction.c:28:13: warning: implicit declaration of function 'assembleInstruction' [-Wimplicit-function-declaration]      mcode = assembleInstruction(tokenizer);)
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owen\Google Drive\bachelor y2\s1\TDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE5FDA1-4123-4096-884D-ED6D195CFF42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47938FB5-FDF4-4291-A4BD-5E8C09A852ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
@@ -737,7 +737,7 @@
   <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,27 +777,27 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed on handling NoOperand instruction , still got bugs on XY, XYSP ,ASP instruction handling fixed implicit declaration of function issue occur on last few commits
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47938FB5-FDF4-4291-A4BD-5E8C09A852ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7EDB24-41C2-468E-A720-A4A6EAE2729D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="14445" yWindow="885" windowWidth="14400" windowHeight="15600" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
   <si>
     <t>ADC</t>
   </si>
@@ -369,13 +369,34 @@
   </si>
   <si>
     <t>assembleASPOperandAndComplexOperand</t>
+  </si>
+  <si>
+    <t>assembleXYSPOperandAndComplexOperand</t>
+  </si>
+  <si>
+    <t>checked once</t>
+  </si>
+  <si>
+    <t>havent decide which module to use</t>
+  </si>
+  <si>
+    <t>todo today</t>
+  </si>
+  <si>
+    <t>checked all</t>
+  </si>
+  <si>
+    <t>Owen STM8 instruction table progress</t>
+  </si>
+  <si>
+    <t>bug</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,8 +404,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +431,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -416,10 +456,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,223 +788,354 @@
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>90</v>
       </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>103</v>
-      </c>
       <c r="B27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -969,7 +1143,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -977,7 +1151,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -985,7 +1159,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -993,7 +1167,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1009,195 +1183,195 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B34" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B34" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B35" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B36" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B37" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B38" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B38" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B39" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B39" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B40" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B41" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B42" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B42" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B43" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B43" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B44" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B45" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B46" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B47" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B48" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B49" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B49" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B50" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B51" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B52" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B53" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B54" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B54" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B55" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B55" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B56" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B56" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1513,7 +1687,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -1521,7 +1695,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>27</v>
       </c>
@@ -1529,57 +1703,73 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="C99" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="C100" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="C101" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B105" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A1:B105">
+  <sortState ref="A1:C105">
     <sortCondition ref="B1:B105"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added custom test assert, finished handling A ,XY, ASP and no operand still need to chg operand.c for the square bracket to handle [$1000.e],[$1000]  ,[$10] and to handle extmem
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7EDB24-41C2-468E-A720-A4A6EAE2729D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEA91A1-7C59-4F2A-B419-41A33762DF10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="885" windowWidth="14400" windowHeight="15600" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="119">
   <si>
     <t>ADC</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>Owen STM8 instruction table progress</t>
-  </si>
-  <si>
-    <t>bug</t>
   </si>
 </sst>
 </file>
@@ -777,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +785,7 @@
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -800,7 +797,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +806,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -822,7 +819,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -835,7 +832,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -848,7 +845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -861,7 +858,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
@@ -870,272 +867,167 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="26" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1143,7 +1035,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1151,7 +1043,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1159,7 +1051,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1059,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1710,9 +1602,7 @@
       <c r="B99" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="C99" s="2"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
@@ -1721,9 +1611,7 @@
       <c r="B100" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="C100" s="2"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
@@ -1732,9 +1620,7 @@
       <c r="B101" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="C101" s="2"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
@@ -1743,9 +1629,7 @@
       <c r="B102" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">

</xml_diff>

<commit_message>
added module to separate function note: still got error on pointers
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEA91A1-7C59-4F2A-B419-41A33762DF10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF5EABE-9E81-4C83-82B7-CDFB7D4CE618}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="-10590" yWindow="5760" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -776,13 +776,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tested custom assert as the custom test_assert is tested as working
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF5EABE-9E81-4C83-82B7-CDFB7D4CE618}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C4A3DE-5DFB-4EBD-81C4-FBF01697814E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10590" yWindow="5760" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="1950" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -475,6 +475,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2567607</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>124239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>587671</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>39300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DABBD933-5CF0-4EB8-A190-E90E52965C56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3180520" y="1648239"/>
+          <a:ext cx="6087325" cy="5630061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -776,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,5 +1711,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added module to support LD , lDR ,ldw still on bug on the module
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C4A3DE-5DFB-4EBD-81C4-FBF01697814E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D921A78-C04A-42DB-8771-168F32EC408D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="123">
   <si>
     <t>ADC</t>
   </si>
@@ -387,6 +387,18 @@
   </si>
   <si>
     <t>Owen STM8 instruction table progress</t>
+  </si>
+  <si>
+    <t>assembleLDOperand</t>
+  </si>
+  <si>
+    <t>assembleLDFOperand</t>
+  </si>
+  <si>
+    <t>assembleLDWOperand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">got bug on LDW ($50,SP),X </t>
   </si>
 </sst>
 </file>
@@ -831,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,27 +1079,27 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1687,23 +1699,32 @@
       </c>
       <c r="C102" s="2"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="B103" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="B104" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B105" s="1"/>
+      <c r="B105" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A1:C105">

</xml_diff>

<commit_message>
added module to support two operand , theres still got bug on bit operation pointer on exception
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D921A78-C04A-42DB-8771-168F32EC408D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C5E7A1-BAE9-43FE-A0F1-4EF437AEA450}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="6495" yWindow="4830" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="122">
   <si>
     <t>ADC</t>
   </si>
@@ -396,9 +396,6 @@
   </si>
   <si>
     <t>assembleLDWOperand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">got bug on LDW ($50,SP),X </t>
   </si>
 </sst>
 </file>
@@ -421,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +449,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -465,13 +468,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,35 +1603,35 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="6" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1721,9 +1725,6 @@
       </c>
       <c r="B105" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the codeInfo to be more module ps: replace at mcode.h the extensioncodeandcode and uint32_t operandExistentFlag with conversion data
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C5E7A1-BAE9-43FE-A0F1-4EF437AEA450}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB615E46-0047-4CFB-9B67-33A7C007D66B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="4830" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="6495" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added function to get flag for different condition now support stackOperation ,incrementDecrement , CompareAndTest, LogicalOperation, bitOperation,Arithmetic Operation, ShiftAndRotates,InterruptManagement,CodecondtionFlagMod and BreakPoint
Ongoing : LoadAndTransfer , ConditionalBitTest&Branch,Unconditionaljump and UnconditionalBranch
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB615E46-0047-4CFB-9B67-33A7C007D66B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F965CF-AF02-49F2-9150-560E21F6AB71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="5430" yWindow="4080" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +455,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -468,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -476,6 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,19 +1418,19 @@
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B67" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="7" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1643,19 +1650,19 @@
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="7" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
operand.c is modified to check if shortptr in shortptr,x is zero then will return bracket x operand and its value finish testing few module (Load&transfer , ArithmeticOperation,Interrupt Management,ConditionCodeFlagModification and BreakPointInstruction
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Students\CWB\TokenizerSkeleton\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8A9CCE-ACDD-42E1-A657-0910E29D3105}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B712794-488B-4CC2-8AE2-FA69E56DE974}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="5430" yWindow="4080" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,13 +498,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -877,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,13 +889,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>101</v>
       </c>
       <c r="D1" s="4"/>
@@ -905,25 +904,25 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>101</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>109</v>
       </c>
       <c r="D3" s="4"/>
@@ -933,13 +932,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>107</v>
       </c>
       <c r="D4" s="4"/>
@@ -949,29 +948,29 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>106</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
       <c r="F5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D6" s="4"/>
@@ -981,58 +980,58 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1081,13 +1080,13 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1427,68 +1426,68 @@
       </c>
     </row>
     <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1537,105 +1536,105 @@
       </c>
     </row>
     <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="C62" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="C63" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+    <row r="65" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="3" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1661,25 +1660,25 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+    <row r="69" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="3" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified operand.c to overcome the shortptrw bracX doesnt throw exception when the flag doesnt support and cause the program to crash when checking the opcode value
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B712794-488B-4CC2-8AE2-FA69E56DE974}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655A2957-2BF6-405E-802B-87D75BCDB10F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="4080" windowWidth="21600" windowHeight="11385" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,24 +1102,24 @@
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1135,13 +1135,13 @@
       </c>
     </row>
     <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1492,46 +1492,46 @@
       </c>
     </row>
     <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>119</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>119</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>119</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>119</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>119</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>119</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>119</v>
       </c>
@@ -1892,46 +1892,46 @@
       </c>
     </row>
     <row r="89" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
instruction set are tested and fully functioning , left some sub module to be tested for better efficiency and stability operand.c and some assemble instruction is modified to overcome some bug experienced during testing please update this file as this is a major commit that improves in first operand checking for instruction that handle two and more operand
</commit_message>
<xml_diff>
--- a/docs/stm8progess.xlsx
+++ b/docs/stm8progess.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TDDtesting\TokenizerSkeleton\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655A2957-2BF6-405E-802B-87D75BCDB10F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32666A41-562F-4638-8F38-383A4893E7D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A2F3971-AAA2-43CC-AD4A-CA3B55AE13E2}"/>
   </bookViews>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D713E5F8-0B0A-4FA3-A210-6B7F77D62830}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,46 +1036,46 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1091,13 +1091,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1124,13 +1124,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1146,282 +1146,282 @@
       </c>
     </row>
     <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="A38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" s="4" t="s">
+      <c r="A46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1683,211 +1683,211 @@
       </c>
     </row>
     <row r="70" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1936,123 +1936,123 @@
       </c>
     </row>
     <row r="93" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C103" s="3" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>